<commit_message>
working with excel book from python
</commit_message>
<xml_diff>
--- a/tim.xlsx
+++ b/tim.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="C3:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,98 +421,208 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>TIm</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>great</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>!</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TIm</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>great</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>!</t>
-        </is>
-      </c>
-    </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TIm</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>great</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>!</t>
+          <t>A1</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TIm</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>great</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>!</t>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>D2</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>end</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A5</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>B5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>C5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>D5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A6</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>C6</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>D6</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>A7</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>D7</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>A8</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>B8</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>C8</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>D8</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>A9</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>B9</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>C9</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>D9</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>A10</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>B10</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>C10</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>D10</t>
         </is>
       </c>
     </row>

</xml_diff>